<commit_message>
standup excel sheetp updated week 2
</commit_message>
<xml_diff>
--- a/Standup_Meeting_StyleSync_G11.xlsx
+++ b/Standup_Meeting_StyleSync_G11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2efca9f02ab0b566/Desktop/school work omegalul/Term 2/5 week term/StyleSync/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="13_ncr:1_{E237BC1A-F91E-DA44-AB6B-3B7A993CB747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1703ADF-AF4A-4818-B2E0-A481162B41BD}"/>
+  <xr:revisionPtr revIDLastSave="132" documentId="13_ncr:1_{E237BC1A-F91E-DA44-AB6B-3B7A993CB747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F151D740-46A8-4E76-87B3-906338FCC416}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{F7BC2121-4CE5-1349-917D-30B6646CA147}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="119">
   <si>
     <t>StyleSync</t>
   </si>
@@ -481,21 +481,10 @@
     <t>Nothing</t>
   </si>
   <si>
-    <t xml:space="preserve">Database Design and </t>
-  </si>
-  <si>
     <t>Git problems</t>
   </si>
   <si>
     <t xml:space="preserve"> Did not work much on project</t>
-  </si>
-  <si>
-    <t>Database Design+D6:D22D9DD6:D23</t>
-  </si>
-  <si>
-    <t>API 
-Branching
- Database</t>
   </si>
   <si>
     <t xml:space="preserve">Branching
@@ -538,6 +527,17 @@
   </si>
   <si>
     <t>Continue working on the design on html pages</t>
+  </si>
+  <si>
+    <t>Database Design</t>
+  </si>
+  <si>
+    <t>Database Design and implementation</t>
+  </si>
+  <si>
+    <t>API 
+Branching
+Database</t>
   </si>
 </sst>
 </file>
@@ -1874,8 +1874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE4008FD-6197-5349-B1C4-61D882D46187}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1957,13 +1957,17 @@
         <v>86</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="E6" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="13"/>
+      <c r="F6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A7" s="36"/>
@@ -1974,13 +1978,17 @@
         <v>87</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="E7" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="14"/>
+      <c r="F7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="37"/>
@@ -1991,13 +1999,17 @@
         <v>88</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E8" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="15"/>
+      <c r="F8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A9" s="35" t="s">
@@ -2010,13 +2022,17 @@
         <v>23</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="E9" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="16"/>
+      <c r="F9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A10" s="36"/>
@@ -2027,13 +2043,17 @@
         <v>23</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E10" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="14"/>
+      <c r="F10" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="47"/>
@@ -2044,13 +2064,17 @@
         <v>23</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E11" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="17"/>
+      <c r="F11" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A12" s="46" t="s">
@@ -2063,13 +2087,17 @@
         <v>89</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="13"/>
+        <v>102</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A13" s="36"/>
@@ -2080,13 +2108,17 @@
         <v>90</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E13" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="14"/>
+      <c r="F13" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="37"/>
@@ -2097,13 +2129,17 @@
         <v>91</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E14" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="15"/>
+      <c r="F14" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="35" t="s">
@@ -2116,13 +2152,17 @@
         <v>92</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E15" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="16"/>
+      <c r="F15" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A16" s="36"/>
@@ -2133,13 +2173,17 @@
         <v>93</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E16" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="14"/>
+      <c r="F16" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="47"/>
@@ -2150,13 +2194,17 @@
         <v>94</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E17" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="F17" s="11"/>
-      <c r="G17" s="17"/>
+      <c r="F17" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A18" s="46" t="s">
@@ -2169,13 +2217,17 @@
         <v>95</v>
       </c>
       <c r="D18" s="28" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="13"/>
+      <c r="F18" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A19" s="36"/>
@@ -2186,13 +2238,17 @@
         <v>96</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E19" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="F19" s="8"/>
-      <c r="G19" s="14"/>
+      <c r="F19" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="37"/>
@@ -2203,13 +2259,17 @@
         <v>97</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E20" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="F20" s="9"/>
-      <c r="G20" s="15"/>
+      <c r="F20" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A21" s="35" t="s">
@@ -2222,13 +2282,17 @@
         <v>98</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E21" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="F21" s="10"/>
-      <c r="G21" s="16"/>
+      <c r="F21" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A22" s="36"/>
@@ -2239,13 +2303,17 @@
         <v>99</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E22" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="F22" s="8"/>
-      <c r="G22" s="14"/>
+      <c r="F22" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="37"/>
@@ -2256,26 +2324,30 @@
         <v>100</v>
       </c>
       <c r="D23" s="32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E23" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="F23" s="9"/>
-      <c r="G23" s="15"/>
+      <c r="F23" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E4:G4"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A4:A5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2569,16 +2641,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2872,16 +2944,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>